<commit_message>
Update deviation from circle table, error in mean calulation!
</commit_message>
<xml_diff>
--- a/Code/Python/Video experiments/settings_deviation_from_circle.xlsx
+++ b/Code/Python/Video experiments/settings_deviation_from_circle.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" state="visible" r:id="rId2"/>
@@ -141,17 +141,17 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.2448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -188,10 +188,10 @@
         <v>-7</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0.88</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -208,10 +208,10 @@
         <v>-5</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>1.92</v>
+        <v>1.29</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>1.04</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -228,10 +228,10 @@
         <v>-3</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>2.53</v>
+        <v>1.52</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>1.44</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -248,10 +248,10 @@
         <v>-5</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>2.17</v>
+        <v>1.21</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>1.48</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -268,10 +268,10 @@
         <v>-3</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>1.96</v>
+        <v>1.85</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>1.47</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,10 +311,10 @@
         <v>-7</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>1.91</v>
+        <v>1.2</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>1.06</v>
+        <v>0.67</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>6</v>
@@ -334,10 +334,10 @@
         <v>-2</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1.63</v>
+        <v>1.01</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>0.93</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -354,10 +354,10 @@
         <v>-4</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>1.36</v>
+        <v>1.42</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>0.98</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -374,10 +374,10 @@
         <v>-4</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>1.61</v>
+        <v>1.11</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>1.04</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -394,10 +394,10 @@
         <v>-4</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>1.23</v>
+        <v>0.79</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>0.6</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -434,10 +434,10 @@
         <v>-3</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>1.36</v>
+        <v>0.9</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>0.72</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -454,10 +454,10 @@
         <v>-2</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>1.3</v>
+        <v>0.81</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>0.72</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,10 +474,10 @@
         <v>-2</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>1.78</v>
+        <v>1.06</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>1.55</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,13 +491,13 @@
         <v>0</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>1.04</v>
+        <v>0.71</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>0.59</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -505,19 +505,19 @@
         <v>0.5</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>-4</v>
+        <v>-7</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>3.45</v>
+        <v>1.69</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>3.44</v>
+        <v>1.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added solar experiment + max for circle
</commit_message>
<xml_diff>
--- a/Code/Python/Video experiments/settings_deviation_from_circle.xlsx
+++ b/Code/Python/Video experiments/settings_deviation_from_circle.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t xml:space="preserve">R</t>
   </si>
@@ -37,10 +37,10 @@
     <t xml:space="preserve">avg std</t>
   </si>
   <si>
-    <t xml:space="preserve">note</t>
+    <t xml:space="preserve">max</t>
   </si>
   <si>
-    <t xml:space="preserve">use measurement 2 and 3</t>
+    <t xml:space="preserve">Solar</t>
   </si>
 </sst>
 </file>
@@ -138,20 +138,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -173,6 +173,9 @@
       <c r="F1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -192,6 +195,9 @@
       </c>
       <c r="F2" s="0" t="n">
         <v>0.67</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>4.3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -213,6 +219,9 @@
       <c r="F3" s="0" t="n">
         <v>0.69</v>
       </c>
+      <c r="G3" s="0" t="n">
+        <v>2.59</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -233,6 +242,9 @@
       <c r="F4" s="0" t="n">
         <v>0.81</v>
       </c>
+      <c r="G4" s="0" t="n">
+        <v>3.95</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -253,8 +265,11 @@
       <c r="F5" s="0" t="n">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="0" t="n">
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>0.5</v>
       </c>
@@ -273,96 +288,106 @@
       <c r="F6" s="0" t="n">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
+      <c r="G6" s="0" t="n">
+        <v>6.08</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>-7</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>0.67</v>
+        <v>50</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>-2</v>
+        <v>-7</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1.01</v>
+        <v>1.2</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>0.57</v>
+        <v>0.67</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>3.03</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>1.42</v>
+        <v>1.01</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>0.92</v>
+        <v>0.57</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>2.64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>33</v>
@@ -374,15 +399,18 @@
         <v>-4</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>1.11</v>
+        <v>1.42</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>0.73</v>
+        <v>0.92</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>4.2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>33</v>
@@ -394,95 +422,111 @@
         <v>-4</v>
       </c>
       <c r="E13" s="0" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E14" s="0" t="n">
         <v>0.79</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F14" s="0" t="n">
         <v>0.37</v>
       </c>
+      <c r="G14" s="0" t="n">
+        <v>1.86</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="0" t="n">
+      <c r="A15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D15" s="0" t="n">
         <v>-3</v>
       </c>
-      <c r="E16" s="0" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>0.45</v>
-      </c>
-    </row>
+      <c r="E15" s="0" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>-2</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>0.81</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>0.43</v>
+        <v>70</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>1.06</v>
+        <v>0.9</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>0.65</v>
+        <v>0.45</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>2.37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>31</v>
@@ -491,33 +535,108 @@
         <v>0</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>0.71</v>
+        <v>0.81</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>0.41</v>
+        <v>0.43</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>2.99</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="B20" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>-7</v>
-      </c>
-      <c r="E20" s="0" t="n">
+      <c r="B22" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E22" s="0" t="n">
         <v>1.69</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F22" s="0" t="n">
         <v>1.23</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>4.53</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>2.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>